<commit_message>
Include Heatrate curve changing every 3 hours, MIP Gap 2.3%
</commit_message>
<xml_diff>
--- a/model/model_inputs_testing_v2.xlsx
+++ b/model/model_inputs_testing_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\Model-1\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC216E7-7984-4A18-884B-82D1D9ACBE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBFC7B1-53F5-469D-8EB8-7CB03731AE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14205" yWindow="0" windowWidth="19395" windowHeight="10200" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>min SoC</t>
   </si>
@@ -171,15 +171,6 @@
     <t>0%-25%</t>
   </si>
   <si>
-    <t>25%-50%</t>
-  </si>
-  <si>
-    <t>50%-75%</t>
-  </si>
-  <si>
-    <t>75%-100%</t>
-  </si>
-  <si>
     <t>Weight</t>
   </si>
   <si>
@@ -211,6 +202,9 @@
   </si>
   <si>
     <t>Number Custumers</t>
+  </si>
+  <si>
+    <t>25%-100</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -1052,7 +1046,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1172,7 +1166,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3">
         <v>0.5</v>
@@ -1249,7 +1243,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3">
         <v>0.5</v>
@@ -1326,7 +1320,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3">
         <v>0.4</v>
@@ -1613,7 +1607,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
@@ -1690,7 +1684,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -1767,7 +1761,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -2056,7 +2050,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3">
         <f>B4</f>
@@ -2157,7 +2151,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3">
         <f>B4</f>
@@ -2258,7 +2252,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -2547,7 +2541,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3">
         <v>0.5</v>
@@ -2624,7 +2618,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3">
         <v>0.5</v>
@@ -2701,7 +2695,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3">
         <v>0.5</v>
@@ -2938,7 +2932,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1">
         <v>150</v>
@@ -3069,7 +3063,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -3145,8 +3139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC45D110-F0D2-4F9D-B0C4-13B38005F879}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -3165,7 +3159,7 @@
         <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3173,7 +3167,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="1">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="C2" s="1">
         <v>0.12</v>
@@ -3187,7 +3181,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="1">
-        <v>0.71</v>
+        <v>0.91</v>
       </c>
       <c r="C3" s="1">
         <v>0.12</v>
@@ -3201,7 +3195,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="1">
-        <v>0.72</v>
+        <v>0.92</v>
       </c>
       <c r="C4" s="1">
         <v>0.13</v>
@@ -3215,7 +3209,7 @@
         <v>27</v>
       </c>
       <c r="B5" s="1">
-        <v>0.73</v>
+        <v>0.93</v>
       </c>
       <c r="C5" s="1">
         <v>0.13</v>
@@ -3229,7 +3223,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="1">
-        <v>0.74</v>
+        <v>0.94</v>
       </c>
       <c r="C6" s="1">
         <v>0.13500000000000001</v>
@@ -3243,7 +3237,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="1">
-        <v>0.75</v>
+        <v>0.95</v>
       </c>
       <c r="C7" s="1">
         <v>0.13900000000000001</v>
@@ -3257,7 +3251,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="1">
-        <v>0.76</v>
+        <v>0.96</v>
       </c>
       <c r="C8" s="1">
         <v>0.14299999999999999</v>
@@ -3271,7 +3265,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="1">
-        <v>0.77</v>
+        <v>0.97</v>
       </c>
       <c r="C9" s="1">
         <v>0.14699999999999999</v>
@@ -3285,7 +3279,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="1">
-        <v>0.78</v>
+        <v>0.98</v>
       </c>
       <c r="C10" s="1">
         <v>0.151</v>
@@ -3299,7 +3293,7 @@
         <v>33</v>
       </c>
       <c r="B11" s="1">
-        <v>0.79</v>
+        <v>0.99</v>
       </c>
       <c r="C11" s="1">
         <v>0.155</v>
@@ -3313,7 +3307,7 @@
         <v>34</v>
       </c>
       <c r="B12" s="1">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1">
         <v>0.159</v>
@@ -3327,7 +3321,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="1">
-        <v>0.81</v>
+        <v>1.01</v>
       </c>
       <c r="C13" s="1">
         <v>0.16300000000000001</v>
@@ -3341,7 +3335,7 @@
         <v>36</v>
       </c>
       <c r="B14" s="1">
-        <v>0.82</v>
+        <v>1.02</v>
       </c>
       <c r="C14" s="1">
         <v>0.16700000000000001</v>
@@ -3355,7 +3349,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="1">
-        <v>0.83</v>
+        <v>1.03</v>
       </c>
       <c r="C15" s="1">
         <v>0.17100000000000001</v>
@@ -3369,7 +3363,7 @@
         <v>38</v>
       </c>
       <c r="B16" s="1">
-        <v>0.84</v>
+        <v>1.04</v>
       </c>
       <c r="C16" s="1">
         <v>0.17499999999999999</v>
@@ -3387,10 +3381,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C056C09-E6BA-453E-9B68-3059E2926BDF}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -3400,57 +3394,25 @@
     <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:2">
       <c r="B1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>40</v>
       </c>
       <c r="B2">
-        <f>(-0.2129*(0.25^3+0^3) +0.6056*(0.25^2+0^2) - 0.5538*(0.25+0) + 0.4067*2)/2</f>
-        <v>0.35473671875000001</v>
-      </c>
-      <c r="G2">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B3">
-        <f>(-0.2129*(0.75^3+0.25^3) +0.6056*(0.75^2+0.25^2) - 0.5538*(0.75+0.25) + 0.4067*2)/2</f>
-        <v>0.27247812500000002</v>
-      </c>
-      <c r="G3">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4">
-        <f>(-0.2129*(0.75^3+0.5^3) +0.6056*(0.75^2+0.5^2) - 0.5538*(0.75+0.5) + 0.4067*2)/2</f>
-        <v>0.24838515625000007</v>
-      </c>
-      <c r="G4">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5">
-        <f>(-0.2129*(1^3+0.75^3) +0.6056*(1^2+0.75^2) - 0.5538*(1+0.75) + 0.4067*2)/2</f>
-        <v>0.24389140625000005</v>
-      </c>
-      <c r="G5">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -3513,12 +3475,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1">
         <v>91</v>
@@ -3526,7 +3488,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1">
         <v>183</v>
@@ -3534,7 +3496,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1">
         <v>91</v>
@@ -3636,7 +3598,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -3713,7 +3675,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -3790,7 +3752,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -3960,7 +3922,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3">
         <v>0.5</v>
@@ -4037,7 +3999,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3">
         <v>0.5</v>
@@ -4114,7 +4076,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3">
         <v>0.4</v>

</xml_diff>

<commit_message>
Finished Heat Rate Function, MIP Gap 1.5%
</commit_message>
<xml_diff>
--- a/model/model_inputs_testing_v2.xlsx
+++ b/model/model_inputs_testing_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\Model-1\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBFC7B1-53F5-469D-8EB8-7CB03731AE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF167FDD-3A8A-4022-BFF7-4875920C9865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14205" yWindow="0" windowWidth="19395" windowHeight="10200" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14205" yWindow="0" windowWidth="19395" windowHeight="10200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -2980,8 +2980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254CDF95-CF95-4796-ABE1-012E5312AEC2}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -3089,16 +3089,16 @@
         <v>20</v>
       </c>
       <c r="B5" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1">
         <v>60</v>
@@ -3112,7 +3112,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="1">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -3121,7 +3121,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="1">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="F6" s="1">
         <v>60</v>
@@ -3139,7 +3139,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC45D110-F0D2-4F9D-B0C4-13B38005F879}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
enlarge customer base, fix major bug with fit
</commit_message>
<xml_diff>
--- a/model/model_inputs_testing_v2.xlsx
+++ b/model/model_inputs_testing_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\Model-1\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF167FDD-3A8A-4022-BFF7-4875920C9865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79351C7B-568C-4CBA-BA5D-6CF744A40495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14205" yWindow="0" windowWidth="19395" windowHeight="10200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19103" yWindow="-98" windowWidth="19395" windowHeight="10395" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,14 @@
     <sheet name="heat_rate" sheetId="8" r:id="rId5"/>
     <sheet name="capacity_steps" sheetId="13" r:id="rId6"/>
     <sheet name="day_weights" sheetId="2" r:id="rId7"/>
-    <sheet name="cap_factors" sheetId="4" r:id="rId8"/>
-    <sheet name="elec_demand (1)" sheetId="3" r:id="rId9"/>
-    <sheet name="elec_demand (2)" sheetId="9" r:id="rId10"/>
-    <sheet name="elec_demand (3)" sheetId="10" r:id="rId11"/>
-    <sheet name="elec_demand (4)" sheetId="11" r:id="rId12"/>
-    <sheet name="elec_demand (5)" sheetId="12" r:id="rId13"/>
+    <sheet name="hist_demand" sheetId="15" r:id="rId8"/>
+    <sheet name="cap_factors" sheetId="4" r:id="rId9"/>
+    <sheet name="elec_demand (1)" sheetId="3" r:id="rId10"/>
+    <sheet name="elec_demand (2)" sheetId="9" r:id="rId11"/>
+    <sheet name="elec_demand (3)" sheetId="10" r:id="rId12"/>
+    <sheet name="elec_demand (4)" sheetId="11" r:id="rId13"/>
+    <sheet name="elec_demand (5)" sheetId="12" r:id="rId14"/>
+    <sheet name="elec_demand (6)" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
   <si>
     <t>min SoC</t>
   </si>
@@ -205,6 +207,42 @@
   </si>
   <si>
     <t>25%-100</t>
+  </si>
+  <si>
+    <t>Type 6</t>
+  </si>
+  <si>
+    <t>demand_elasticity</t>
+  </si>
+  <si>
+    <t>perc_share</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>demand</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>H6</t>
   </si>
 </sst>
 </file>
@@ -1012,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1024,9 +1062,10 @@
     <col min="2" max="2" width="10.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1048,8 +1087,11 @@
       <c r="G1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0.2</v>
       </c>
@@ -1070,6 +1112,9 @@
       </c>
       <c r="G2" s="1">
         <v>0.05</v>
+      </c>
+      <c r="H2" s="1">
+        <v>-0.12130000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1078,6 +1123,449 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABED9F3-A079-4BB6-8141-C898B88CBE8C}">
+  <dimension ref="A1:Y31"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="25" width="6.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1</v>
+      </c>
+      <c r="N2" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="O2" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="P2" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="S2" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="T2" s="3">
+        <v>2</v>
+      </c>
+      <c r="U2" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="V2" s="3">
+        <v>2</v>
+      </c>
+      <c r="W2" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="X2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="M3" s="3">
+        <v>1</v>
+      </c>
+      <c r="N3" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="O3" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="P3" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="R3" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="S3" s="3">
+        <v>2</v>
+      </c>
+      <c r="T3" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="U3" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="V3" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="W3" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="X3" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="O4" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="P4" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="R4" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="S4" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="T4" s="3">
+        <v>2.7</v>
+      </c>
+      <c r="U4" s="3">
+        <v>3</v>
+      </c>
+      <c r="V4" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="W4" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="X4" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="2"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="2"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="2"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="2"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="2"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="2"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867F374D-6AFF-43B6-B370-B2ECC1DAC459}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
@@ -1518,7 +2006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A01985ED-3AF2-4182-BB5C-CF8628DEF823}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
@@ -1961,7 +2449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F25FDCC-0E53-468A-95CC-401F964650F2}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
@@ -2452,8 +2940,451 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE540155-C042-4D87-9ACA-1F490BE78401}">
+  <dimension ref="A1:Y31"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="25" width="6.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="J2" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="K2" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="L2" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="M2" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="N2" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="O2" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="P2" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="R2" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="S2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="T2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="U2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="V2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="W2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="X2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="J3" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="K3" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="L3" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="M3" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="N3" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="O3" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="P3" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="R3" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="S3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="T3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="U3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="V3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="W3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="X3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="J4" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="K4" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="L4" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="M4" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="N4" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="O4" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="P4" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="R4" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="S4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="V4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="X4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="2"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="2"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="2"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="2"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="2"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="2"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C93B0C-716A-4CFD-8E38-BA44799D71A5}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2897,10 +3828,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E688FB98-37F3-4971-B4CD-1E6A7262204F}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2913,7 +3844,7 @@
     <col min="6" max="6" width="8.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" t="s">
         <v>6</v>
       </c>
@@ -2929,28 +3860,34 @@
       <c r="F1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="1">
-        <v>150</v>
+        <v>600</v>
       </c>
       <c r="C2" s="1">
-        <v>100</v>
+        <v>550</v>
       </c>
       <c r="D2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>160</v>
+      </c>
+      <c r="G2" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2958,16 +3895,24 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>15</v>
+        <v>2.7</v>
       </c>
       <c r="D3" s="1">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
         <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2980,8 +3925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254CDF95-CF95-4796-ABE1-012E5312AEC2}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -3509,6 +4454,137 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243AAE38-9D6F-4012-8878-02E57E613A97}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>100000</v>
+      </c>
+      <c r="C2">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="G2">
+        <f xml:space="preserve"> SUM('elec_demand (1)'!$B2:$Y2)</f>
+        <v>25.300000000000004</v>
+      </c>
+      <c r="H2">
+        <f xml:space="preserve"> SUM('elec_demand (2)'!$B2:$Y2)</f>
+        <v>25.300000000000004</v>
+      </c>
+      <c r="I2">
+        <f xml:space="preserve"> SUM('elec_demand (2)'!$B2:$Y2)</f>
+        <v>25.300000000000004</v>
+      </c>
+      <c r="J2">
+        <f xml:space="preserve"> SUM('elec_demand (3)'!$B2:$Y2)</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f xml:space="preserve"> SUM('elec_demand (4)'!$B2:$Y2)</f>
+        <v>141</v>
+      </c>
+      <c r="L2">
+        <f xml:space="preserve"> SUM('elec_demand (5)'!$B2:$Y2)</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="G3">
+        <f xml:space="preserve"> SUM('elec_demand (1)'!B3:Y3)</f>
+        <v>27.800000000000004</v>
+      </c>
+      <c r="H3">
+        <f xml:space="preserve"> SUM('elec_demand (2)'!$B3:$Y3)</f>
+        <v>27.800000000000004</v>
+      </c>
+      <c r="I3">
+        <f xml:space="preserve"> SUM('elec_demand (2)'!$B3:$Y3)</f>
+        <v>27.800000000000004</v>
+      </c>
+      <c r="J3">
+        <f xml:space="preserve"> SUM('elec_demand (3)'!$B3:$Y3)</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f xml:space="preserve"> SUM('elec_demand (4)'!$B3:$Y3)</f>
+        <v>86</v>
+      </c>
+      <c r="L3">
+        <f xml:space="preserve"> SUM('elec_demand (5)'!$B3:$Y3)</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="G4">
+        <f xml:space="preserve"> SUM('elec_demand (1)'!B4:Y4)</f>
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <f xml:space="preserve"> SUM('elec_demand (2)'!$B4:$Y4)</f>
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <f xml:space="preserve"> SUM('elec_demand (2)'!$B4:$Y4)</f>
+        <v>30</v>
+      </c>
+      <c r="J4">
+        <f xml:space="preserve"> SUM('elec_demand (3)'!$B4:$Y4)</f>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f xml:space="preserve"> SUM('elec_demand (4)'!$B4:$Y4)</f>
+        <v>31</v>
+      </c>
+      <c r="L4">
+        <f xml:space="preserve"> SUM('elec_demand (5)'!$B4:$Y4)</f>
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE7DE72-C341-45B3-B73B-C7F84D832AAF}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
@@ -3831,447 +4907,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABED9F3-A079-4BB6-8141-C898B88CBE8C}">
-  <dimension ref="A1:Y31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
-  <cols>
-    <col min="2" max="25" width="6.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-      <c r="N1">
-        <v>13</v>
-      </c>
-      <c r="O1">
-        <v>14</v>
-      </c>
-      <c r="P1">
-        <v>15</v>
-      </c>
-      <c r="Q1">
-        <v>16</v>
-      </c>
-      <c r="R1">
-        <v>17</v>
-      </c>
-      <c r="S1">
-        <v>18</v>
-      </c>
-      <c r="T1">
-        <v>19</v>
-      </c>
-      <c r="U1">
-        <v>20</v>
-      </c>
-      <c r="V1">
-        <v>21</v>
-      </c>
-      <c r="W1">
-        <v>22</v>
-      </c>
-      <c r="X1">
-        <v>23</v>
-      </c>
-      <c r="Y1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="J2" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="K2" s="3">
-        <v>1</v>
-      </c>
-      <c r="L2" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="M2" s="3">
-        <v>1</v>
-      </c>
-      <c r="N2" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="O2" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="P2" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>1</v>
-      </c>
-      <c r="R2" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="S2" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="T2" s="3">
-        <v>2</v>
-      </c>
-      <c r="U2" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="V2" s="3">
-        <v>2</v>
-      </c>
-      <c r="W2" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="X2" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="Y2" s="3">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="J3" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="K3" s="3">
-        <v>1</v>
-      </c>
-      <c r="L3" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="M3" s="3">
-        <v>1</v>
-      </c>
-      <c r="N3" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="O3" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="P3" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="R3" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="S3" s="3">
-        <v>2</v>
-      </c>
-      <c r="T3" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="U3" s="3">
-        <v>2.6</v>
-      </c>
-      <c r="V3" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="W3" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="X3" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="Y3" s="3">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="H4" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="J4" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="K4" s="3">
-        <v>1</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="M4" s="3">
-        <v>1</v>
-      </c>
-      <c r="N4" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="O4" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="P4" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="R4" s="3">
-        <v>1.9</v>
-      </c>
-      <c r="S4" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="T4" s="3">
-        <v>2.7</v>
-      </c>
-      <c r="U4" s="3">
-        <v>3</v>
-      </c>
-      <c r="V4" s="3">
-        <v>2.6</v>
-      </c>
-      <c r="W4" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="X4" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Y4" s="3">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
progress with Unmet Demand
</commit_message>
<xml_diff>
--- a/model/model_inputs_testing_v2.xlsx
+++ b/model/model_inputs_testing_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\Model-1\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79351C7B-568C-4CBA-BA5D-6CF744A40495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF3D89B-C99D-4B52-B869-6DE86E7D213A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19103" yWindow="-98" windowWidth="19395" windowHeight="10395" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10395" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,17 @@
     <sheet name="tech" sheetId="6" r:id="rId3"/>
     <sheet name="tariffs" sheetId="7" r:id="rId4"/>
     <sheet name="heat_rate" sheetId="8" r:id="rId5"/>
-    <sheet name="capacity_steps" sheetId="13" r:id="rId6"/>
-    <sheet name="day_weights" sheetId="2" r:id="rId7"/>
-    <sheet name="hist_demand" sheetId="15" r:id="rId8"/>
-    <sheet name="cap_factors" sheetId="4" r:id="rId9"/>
-    <sheet name="elec_demand (1)" sheetId="3" r:id="rId10"/>
-    <sheet name="elec_demand (2)" sheetId="9" r:id="rId11"/>
-    <sheet name="elec_demand (3)" sheetId="10" r:id="rId12"/>
-    <sheet name="elec_demand (4)" sheetId="11" r:id="rId13"/>
-    <sheet name="elec_demand (5)" sheetId="12" r:id="rId14"/>
-    <sheet name="elec_demand (6)" sheetId="14" r:id="rId15"/>
+    <sheet name="elec_price" sheetId="16" r:id="rId6"/>
+    <sheet name="capacity_steps" sheetId="13" r:id="rId7"/>
+    <sheet name="day_weights" sheetId="2" r:id="rId8"/>
+    <sheet name="hist_demand" sheetId="15" r:id="rId9"/>
+    <sheet name="cap_factors" sheetId="4" r:id="rId10"/>
+    <sheet name="elec_demand (1)" sheetId="3" r:id="rId11"/>
+    <sheet name="elec_demand (2)" sheetId="9" r:id="rId12"/>
+    <sheet name="elec_demand (3)" sheetId="10" r:id="rId13"/>
+    <sheet name="elec_demand (4)" sheetId="11" r:id="rId14"/>
+    <sheet name="elec_demand (5)" sheetId="12" r:id="rId15"/>
+    <sheet name="elec_demand (6)" sheetId="14" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
   <si>
     <t>min SoC</t>
   </si>
@@ -1123,6 +1124,331 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE7DE72-C341-45B3-B73B-C7F84D832AAF}">
+  <dimension ref="A1:Y4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="25" width="5.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="S2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="T2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="U2" s="1">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1">
+        <v>0</v>
+      </c>
+      <c r="W2" s="1">
+        <v>0</v>
+      </c>
+      <c r="X2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1">
+        <v>0</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0</v>
+      </c>
+      <c r="V4" s="1">
+        <v>0</v>
+      </c>
+      <c r="W4" s="1">
+        <v>0</v>
+      </c>
+      <c r="X4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ABED9F3-A079-4BB6-8141-C898B88CBE8C}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
@@ -1565,7 +1891,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867F374D-6AFF-43B6-B370-B2ECC1DAC459}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
@@ -2006,7 +2332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A01985ED-3AF2-4182-BB5C-CF8628DEF823}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
@@ -2449,7 +2775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F25FDCC-0E53-468A-95CC-401F964650F2}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
@@ -2940,7 +3266,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE540155-C042-4D87-9ACA-1F490BE78401}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
@@ -3383,7 +3709,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C93B0C-716A-4CFD-8E38-BA44799D71A5}">
   <dimension ref="A1:Y31"/>
   <sheetViews>
@@ -4366,6 +4692,51 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E9053E1-71CC-49BE-991D-93373BCD5FC7}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>3.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDB5C9E-DDE6-4406-A1BA-E0B87BADDE72}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -4408,7 +4779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB9A018-F4D8-4049-8785-D914448B1EBA}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -4453,12 +4824,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243AAE38-9D6F-4012-8878-02E57E613A97}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -4494,13 +4865,13 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>100000</v>
+        <v>110314</v>
       </c>
       <c r="C2">
-        <v>0.38200000000000001</v>
+        <v>0.37</v>
       </c>
       <c r="G2">
         <f xml:space="preserve"> SUM('elec_demand (1)'!$B2:$Y2)</f>
@@ -4528,6 +4899,15 @@
       </c>
     </row>
     <row r="3" spans="1:12">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>101450</v>
+      </c>
+      <c r="C3">
+        <v>0.37</v>
+      </c>
       <c r="G3">
         <f xml:space="preserve"> SUM('elec_demand (1)'!B3:Y3)</f>
         <v>27.800000000000004</v>
@@ -4554,6 +4934,15 @@
       </c>
     </row>
     <row r="4" spans="1:12">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>126000</v>
+      </c>
+      <c r="C4">
+        <v>0.37</v>
+      </c>
       <c r="G4">
         <f xml:space="preserve"> SUM('elec_demand (1)'!B4:Y4)</f>
         <v>30</v>
@@ -4582,329 +4971,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE7DE72-C341-45B3-B73B-C7F84D832AAF}">
-  <dimension ref="A1:Y4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="25" width="5.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-      <c r="N1">
-        <v>13</v>
-      </c>
-      <c r="O1">
-        <v>14</v>
-      </c>
-      <c r="P1">
-        <v>15</v>
-      </c>
-      <c r="Q1">
-        <v>16</v>
-      </c>
-      <c r="R1">
-        <v>17</v>
-      </c>
-      <c r="S1">
-        <v>18</v>
-      </c>
-      <c r="T1">
-        <v>19</v>
-      </c>
-      <c r="U1">
-        <v>20</v>
-      </c>
-      <c r="V1">
-        <v>21</v>
-      </c>
-      <c r="W1">
-        <v>22</v>
-      </c>
-      <c r="X1">
-        <v>23</v>
-      </c>
-      <c r="Y1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="L2" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="M2" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="N2" s="1">
-        <v>1</v>
-      </c>
-      <c r="O2" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="P2" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="R2" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="S2" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="T2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="U2" s="1">
-        <v>0</v>
-      </c>
-      <c r="V2" s="1">
-        <v>0</v>
-      </c>
-      <c r="W2" s="1">
-        <v>0</v>
-      </c>
-      <c r="X2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="M3" s="1">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="S3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="T3" s="1">
-        <v>0</v>
-      </c>
-      <c r="U3" s="1">
-        <v>0</v>
-      </c>
-      <c r="V3" s="1">
-        <v>0</v>
-      </c>
-      <c r="W3" s="1">
-        <v>0</v>
-      </c>
-      <c r="X3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="M4" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="N4" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="O4" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="R4" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="S4" s="1">
-        <v>0</v>
-      </c>
-      <c r="T4" s="1">
-        <v>0</v>
-      </c>
-      <c r="U4" s="1">
-        <v>0</v>
-      </c>
-      <c r="V4" s="1">
-        <v>0</v>
-      </c>
-      <c r="W4" s="1">
-        <v>0</v>
-      </c>
-      <c r="X4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
remove energy desc. variables, add new input file
</commit_message>
<xml_diff>
--- a/model/model_inputs_testing_v2.xlsx
+++ b/model/model_inputs_testing_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jakob\PycharmProjects\Model-1\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF3D89B-C99D-4B52-B869-6DE86E7D213A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B91920B-BBC1-49BB-BFE1-158E26DD7989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10395" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5310" yWindow="1140" windowWidth="21600" windowHeight="11145" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="64">
   <si>
     <t>min SoC</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>Owned Batteries</t>
-  </si>
-  <si>
-    <t>Owned Batteries Energy</t>
   </si>
   <si>
     <t>Diesel Price</t>
@@ -1054,7 +1051,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1086,10 +1083,10 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1106,7 +1103,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1">
         <v>24</v>
@@ -1213,7 +1210,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -1290,7 +1287,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -1367,7 +1364,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -1537,7 +1534,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3">
         <v>0.5</v>
@@ -1614,7 +1611,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3">
         <v>0.5</v>
@@ -1691,7 +1688,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3">
         <v>0.4</v>
@@ -1980,7 +1977,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3">
         <v>0.5</v>
@@ -2057,7 +2054,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3">
         <v>0.5</v>
@@ -2134,7 +2131,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3">
         <v>0.4</v>
@@ -2421,7 +2418,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
@@ -2498,7 +2495,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3">
         <v>0</v>
@@ -2575,7 +2572,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -2864,7 +2861,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3">
         <f>B4</f>
@@ -2965,7 +2962,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3">
         <f>B4</f>
@@ -3066,7 +3063,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -3355,7 +3352,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3">
         <v>0.5</v>
@@ -3432,7 +3429,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3">
         <v>0.5</v>
@@ -3509,7 +3506,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3">
         <v>0.5</v>
@@ -3798,7 +3795,7 @@
     </row>
     <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3">
         <v>0.5</v>
@@ -3875,7 +3872,7 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3">
         <v>0.5</v>
@@ -3952,7 +3949,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3">
         <v>0.5</v>
@@ -4187,12 +4184,12 @@
         <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1">
         <v>600</v>
@@ -4238,7 +4235,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -4249,10 +4246,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254CDF95-CF95-4796-ABE1-012E5312AEC2}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -4297,10 +4294,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="F2" s="1">
         <v>20</v>
@@ -4334,7 +4331,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -4349,10 +4346,10 @@
         <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4369,7 +4366,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="F5" s="1">
         <v>60</v>
@@ -4378,28 +4375,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1">
-        <v>5</v>
-      </c>
-      <c r="E6" s="1">
-        <v>350</v>
-      </c>
-      <c r="F6" s="1">
-        <v>60</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
+    <row r="13" spans="1:7">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4410,8 +4392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC45D110-F0D2-4F9D-B0C4-13B38005F879}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -4424,18 +4406,18 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
-        <v>23</v>
-      </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1">
         <v>0.9</v>
@@ -4449,10 +4431,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1">
-        <v>0.91</v>
+        <v>0.9</v>
       </c>
       <c r="C3" s="1">
         <v>0.12</v>
@@ -4463,10 +4445,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1">
-        <v>0.92</v>
+        <v>0.9</v>
       </c>
       <c r="C4" s="1">
         <v>0.13</v>
@@ -4477,10 +4459,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1">
-        <v>0.93</v>
+        <v>0.9</v>
       </c>
       <c r="C5" s="1">
         <v>0.13</v>
@@ -4491,10 +4473,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1">
-        <v>0.94</v>
+        <v>0.9</v>
       </c>
       <c r="C6" s="1">
         <v>0.13500000000000001</v>
@@ -4505,10 +4487,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="C7" s="1">
         <v>0.13900000000000001</v>
@@ -4519,10 +4501,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1">
-        <v>0.96</v>
+        <v>0.9</v>
       </c>
       <c r="C8" s="1">
         <v>0.14299999999999999</v>
@@ -4533,10 +4515,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1">
-        <v>0.97</v>
+        <v>0.9</v>
       </c>
       <c r="C9" s="1">
         <v>0.14699999999999999</v>
@@ -4547,10 +4529,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1">
-        <v>0.98</v>
+        <v>0.9</v>
       </c>
       <c r="C10" s="1">
         <v>0.151</v>
@@ -4561,10 +4543,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1">
-        <v>0.99</v>
+        <v>0.9</v>
       </c>
       <c r="C11" s="1">
         <v>0.155</v>
@@ -4575,10 +4557,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="C12" s="1">
         <v>0.159</v>
@@ -4589,10 +4571,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1">
-        <v>1.01</v>
+        <v>0.9</v>
       </c>
       <c r="C13" s="1">
         <v>0.16300000000000001</v>
@@ -4603,10 +4585,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1">
-        <v>1.02</v>
+        <v>0.9</v>
       </c>
       <c r="C14" s="1">
         <v>0.16700000000000001</v>
@@ -4617,10 +4599,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1">
-        <v>1.03</v>
+        <v>0.9</v>
       </c>
       <c r="C15" s="1">
         <v>0.17100000000000001</v>
@@ -4631,10 +4613,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1">
-        <v>1.04</v>
+        <v>0.9</v>
       </c>
       <c r="C16" s="1">
         <v>0.17499999999999999</v>
@@ -4667,12 +4649,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>0.35</v>
@@ -4680,7 +4662,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3">
         <v>0.25</v>
@@ -4695,7 +4677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E9053E1-71CC-49BE-991D-93373BCD5FC7}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -4703,7 +4685,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -4791,12 +4773,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1">
         <v>91</v>
@@ -4804,7 +4786,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1">
         <v>183</v>
@@ -4812,7 +4794,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1">
         <v>91</v>
@@ -4836,31 +4818,31 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>58</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>60</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>61</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>62</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>63</v>
-      </c>
-      <c r="L1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:12">

</xml_diff>